<commit_message>
import excel in angular (show data as json)
</commit_message>
<xml_diff>
--- a/import attendee list.xlsx
+++ b/import attendee list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\event_organizing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A668BAA-0049-4954-8C14-980F33421A5F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28C60FB-D118-4D39-AB5C-9A8DE6933DB9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>No.</t>
   </si>
@@ -57,35 +57,38 @@
     <t>Address</t>
   </si>
   <si>
-    <t>&lt;optional&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sample address, optional&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sample.email, required&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sample, required&gt;</t>
-  </si>
-  <si>
-    <t>&lt;male, optional&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sample ic/passport no., optional&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sample phone number, optional&gt;</t>
-  </si>
-  <si>
-    <t>&lt;sample org., optional&gt;</t>
+    <t>Tan Zhang En</t>
+  </si>
+  <si>
+    <t>zhangen69@gmail.com</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>940830-01-6651</t>
+  </si>
+  <si>
+    <t>019-7765290</t>
+  </si>
+  <si>
+    <t>Soo De Xiang</t>
+  </si>
+  <si>
+    <t>dexiang@gmail.com</t>
+  </si>
+  <si>
+    <t>980122-01-6412</t>
+  </si>
+  <si>
+    <t>012-1325418</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +101,14 @@
       <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -118,13 +129,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -403,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -458,36 +472,48 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
+      <c r="F3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{1F339EBC-479C-48FC-A98D-54F66602383F}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{09DA114D-F6F7-4AE7-861B-C97B201A0A0E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>